<commit_message>
wybitnie celna i celna obsłużone
</commit_message>
<xml_diff>
--- a/SpecjalizacjeDoZrobienia.xlsx
+++ b/SpecjalizacjeDoZrobienia.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -31,9 +31,6 @@
     <t xml:space="preserve">umiejka1</t>
   </si>
   <si>
-    <t xml:space="preserve">warunki</t>
-  </si>
-  <si>
     <t xml:space="preserve">opis</t>
   </si>
   <si>
@@ -43,16 +40,13 @@
     <t xml:space="preserve">umiejka3</t>
   </si>
   <si>
-    <t xml:space="preserve">umiejka4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ULT</t>
+    <t xml:space="preserve">ult</t>
   </si>
   <si>
     <t xml:space="preserve">Bron boczna</t>
   </si>
   <si>
-    <t xml:space="preserve">obsluga broni, refleks, strzelectwo, prowadzenie pojazdu, ukrywanie, zreczne palce </t>
+    <t xml:space="preserve">obsluga broni, refleks,  strzelectwo, prowadzenie pojazdu, ukrywanie, zreczne palce</t>
   </si>
   <si>
     <t xml:space="preserve">Wprawa
@@ -62,44 +56,22 @@
     <t xml:space="preserve">Pistolet, Rewolwer, Pistolet maszynowy, Jednoręczna, Kompaktowa</t>
   </si>
   <si>
-    <t xml:space="preserve">Możesz zamienić wynik wyrzucony na jednej z kości podczas testu Strzelectwa na liczbę równą poziomowi tej umiejętności podczas strzelania z broni z którąś z zasad Pistolet, Rewolwer, Pistolet maszynowy, Jednoręczna, Kompaktowa. Nie łączy się z umiejętnościami o tej samej nazwie z innych specjalizacji.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zasieg 2, Z biodra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pistolet, Rewolwer, Pistolet maszynowy, Jednoręczna, Kompaktowa.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">Ślepy ostrzał
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve"> Za każdy poziom tej umiejętności, zwiększ przyrost zasięgu z biodra o 2m dla broni z którąś z zasad Pistolet, Rewolwer, Pistolet maszynowy, Jednoręczna, Kompaktowa. </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Umiejetnosc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dobycie broni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Predyspozycje</t>
+    <t xml:space="preserve">Slepy ostrzal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każdy poziom tej umiejętności, zwiększ przyrost zasięgu strzelania z biodra o 2m dla broni z którąś z zasad Pistolet, Rewolwer, Pistolet maszynowy, Jednoręczna, Kompaktowa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szybki rewolwerowiec (Zr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zdając test tej umiejętności, możesz oddać strzał w fazie, w której dobywasz broń. Deklarujesz to przed dobyciem. Poziom trudności 5 dla Pistolet, Rewolwer, Jednoręczna, 10 dla Pistolet maszynowy, Kompaktowa. Jak nie zdasz, nie trafiasz (Ale pamiętaj że strzał oddałeś). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ruchomy strzelec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">za każdy poziom tej umiejętności zmniejsz karę za ruch podczas strzelania o 1 dla broni z zasadą Pistolet, Rewolwer, Pistolet maszynowy, Jednoręczna, Kompaktowa.</t>
   </si>
   <si>
     <t xml:space="preserve">Karabiny</t>
@@ -108,21 +80,76 @@
     <t xml:space="preserve">obsluga broni, refleks, strzelectwo, zmysl bitewny, spostrzeganie, sprawnosc fizyczna </t>
   </si>
   <si>
+    <t xml:space="preserve"> z broni zasilanej nabojami pośrednimi i karabinowymi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kontroler spustu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W momencie strzelania w trybie full auto z broni zasilanej nabojami pośrednimi i karabinowymi, gdy są naboje wystrzelone nie generujące kości obrażeń, zużywasz o tyle mniej amunicji, ile masz poziomów w tej umiejętności. Nigdy nie możesz zużyć mniej naboi niż masz trafień. Dodatkowo, na 6 poziomie dostajesz możliwość wystrzelenia 2 serii w fazie.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szybki spust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za karę w wysokości ⅓ odrzutu (zaokrąglając na niekorzyść, ale po modyfikatorach), możesz strzelić dodatkowy raz w trybie pojedynczym z broni zasilanej nabojami pośrednimi i karabinowymi, w liczbie nie większej niż poziom tej umiejętności dzielone przez 3 (zaokrąglając w dół). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mistrz karabinów: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">zmniejsz dodatkowy odrzut o 1 dla trybów samoczynne i serie (ale nigdy poniżej wartości pojedyńczego odrzutu po modyfikatorach). Dodatkowo jeśli osiągnąłeś 3. poziom tej umiejętności, to modyfikuje zasadę “Dokładne celowanie” zmniejszając wymagane przekroczenie rzutu na trafienie z 3 do 2. Jeśli posiadasz 6. poziom tej umiejętności to zmniejszasz wymagane przekroczenie rzutu na trafienie z 3 do 1. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Bron krotka</t>
   </si>
   <si>
     <t xml:space="preserve">obsluga broni, refleks, strzelectwo, zmysl bitewny, ukrywanie, zreczne palce </t>
   </si>
   <si>
-    <t xml:space="preserve">Broń awaryjna w walce wręcz
-W walce wręcz zamiast ataku możesz strzelać z broni z zasadą Pistolet, Rewolwer, Pistolet maszynowy, Jednoręczna, Kompaktowa. Zwiększasz odrzut podwójnie. Ten strzał musi być wykonany z modyfikatorem „Z biodra”. Używasz wtedy poziomu tej umiejętności jako poziomu kości ataku (nie sumuje się z Wprawą).  
-Jest chujowa - po reworku walki wrecz jest bardzo słabo (chociazby zeby nie zamieniac kosci ataku na poziom tego skilla)</t>
+    <t xml:space="preserve">Pistolet, Rewolwer, lub Działo ręczne </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perfekcyjne zgranie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">za każdy poziom tej umiejętności, na kolejnych przyrostach zasięgów, zasada pistolet, rewolwer, działo reczne nie obowiązuje w kontekście mnożnika kary za zasięg. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za karę podwójnego odrzutu (po redukcjach), możesz strzelić dodatkowy raz w trybie Pojedynczy, w liczbie nie większej niż poziom tej umiejętności dzielone przez 3. Tylko dla broni z broni zasilaną amunicją pistoletową i rewolwerową. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jednoręki bandyta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Każdy poziom redukuje kary podczas strzelania z broni z zasadą Pistolet, Rewolwer, lub Działo ręczne z jednej ręki o 1. </t>
   </si>
   <si>
     <t xml:space="preserve">Karabiny maszynowe</t>
   </si>
   <si>
     <t xml:space="preserve">obsluga broni, strzelectwo, spostrzeganie, sprawnosc fizyczna, ukrywanie, zawod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siłacz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każdy poziom tej umiejętności zmniejsz karę z zasady specjalnej Kobyła oraz Ciężka o 1 (max do 0) podczas strzelania z broni z zasadą KM oraz wszelkich karabinów zasilanych taśmą. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ściana ognia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dodatkowa premia do ataku strzelając full auto z broni z zasadą KM oraz wszelkich karabinów zasilanych taśmą. Musisz się rozstawić (skorzystać z dwójnogu) aby móc skorzystać z tej </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zaporowe przerażenie (Krz)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W tym przypadku zabić można przy okazji. Ty zabijasz przede wszystkim ducha walki. Strzelając ogniem samoczynnym, możesz stwierdzić że chcesz przerazić przeciwników ostrzałem (musisz strzelać w kierunku przeciwnika, ale niekoniecznie bezpośrednio w niego). Zdanie tego testu na 5/10/15/20, oznacza że przeciwnik traci 1,3,5,7 dodatkowych punktów wytrwałości. Ponadto jeśli przeciwnik może ponad walkę wybrać ucieczkę to to zrobi.</t>
   </si>
   <si>
     <t xml:space="preserve">Karabiny wyborowe</t>
@@ -388,7 +415,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -420,17 +447,19 @@
   </sheetPr>
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="131.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="97.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="51.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -443,292 +472,337 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="J1" s="4"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="152.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="J2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="E3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" customFormat="false" ht="135.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
+      <c r="H4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="N4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="8.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>66</v>
+        <v>81</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>68</v>
+        <v>83</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>70</v>
+        <v>85</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
przygotowanie kary za ruch
</commit_message>
<xml_diff>
--- a/SpecjalizacjeDoZrobienia.xlsx
+++ b/SpecjalizacjeDoZrobienia.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="88">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t xml:space="preserve">refleks, skupienie, strzelectwo, spostrzeganie, ukrywanie, dyscyplina naukowa </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snajperka i Duży kaliber </t>
   </si>
   <si>
     <t xml:space="preserve">Luki i kusze</t>
@@ -447,8 +450,8 @@
   </sheetPr>
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -627,182 +630,187 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="8.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prepared for new Specialisations
</commit_message>
<xml_diff>
--- a/SpecjalizacjeDoZrobienia.xlsx
+++ b/SpecjalizacjeDoZrobienia.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="90">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -80,7 +80,7 @@
     <t xml:space="preserve">obsluga broni, refleks, strzelectwo, zmysl bitewny, spostrzeganie, sprawnosc fizyczna </t>
   </si>
   <si>
-    <t xml:space="preserve"> z broni zasilanej nabojami pośrednimi i karabinowymi </t>
+    <t xml:space="preserve">Amunicja: pośrednia, karabinowa </t>
   </si>
   <si>
     <t xml:space="preserve">Kontroler spustu</t>
@@ -107,7 +107,7 @@
     <t xml:space="preserve">obsluga broni, refleks, strzelectwo, zmysl bitewny, ukrywanie, zreczne palce </t>
   </si>
   <si>
-    <t xml:space="preserve">Pistolet, Rewolwer, lub Działo ręczne </t>
+    <t xml:space="preserve">Pistolet, Rewolwer, Działo ręczne </t>
   </si>
   <si>
     <t xml:space="preserve">Perfekcyjne zgranie</t>
@@ -167,10 +167,16 @@
     <t xml:space="preserve">obsluga broni, refleks, strzelectwo, spostrzeganie, sprawnosc fizyczna, zreczne palce </t>
   </si>
   <si>
+    <t xml:space="preserve">łuk, Kusza</t>
+  </si>
+  <si>
     <t xml:space="preserve">Materialy wybuchowe</t>
   </si>
   <si>
     <t xml:space="preserve">obsluga broni, strzelectwo, spostrzeganie, sprawnosc fizyczna, dyscyplina naukowa, zawod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wprawa </t>
   </si>
   <si>
     <t xml:space="preserve">Pistolety maszynowe</t>
@@ -450,14 +456,14 @@
   </sheetPr>
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="97.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="97.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.64"/>
@@ -510,7 +516,7 @@
       <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -648,173 +654,184 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="8.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
strange error durring loading first bullet into chamber... redo equipment, and specialisations partly ready.
</commit_message>
<xml_diff>
--- a/SpecjalizacjeDoZrobienia.xlsx
+++ b/SpecjalizacjeDoZrobienia.xlsx
@@ -20,12 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="91">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
   <si>
     <t xml:space="preserve">umiejętności powiązane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">poziom</t>
   </si>
   <si>
     <t xml:space="preserve">umiejka1</t>
@@ -399,7 +402,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -422,10 +425,6 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -454,25 +453,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="97.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="51.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="11" style="0" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="44.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="33.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="51.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="15" style="0" width="11.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -482,361 +481,713 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="3"/>
+      <c r="L1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="4"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="C3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="K3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="L3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>25</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="5" t="s">
         <v>28</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="L4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
+      <c r="N4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
         <v>36</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="K5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="L5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>42</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5" t="s">
         <v>45</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
+        <v>48</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>48</v>
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C8" s="0" t="s">
         <v>51</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>51</v>
+      <c r="F9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="C13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="C15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="8.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L18" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
-        <v>72</v>
+      <c r="A19" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L20" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L22" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L23" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
-        <v>82</v>
+      <c r="A24" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L29" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="R4:U4"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
did specs into file. now ith's time to read it as whole, and use.
</commit_message>
<xml_diff>
--- a/SpecjalizacjeDoZrobienia.xlsx
+++ b/SpecjalizacjeDoZrobienia.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="251">
   <si>
     <t xml:space="preserve">nazwa</t>
   </si>
@@ -164,6 +164,24 @@
     <t xml:space="preserve">Snajperka, Duży kaliber </t>
   </si>
   <si>
+    <t xml:space="preserve">Precyzyjne kierowanie kulami</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każdą fazę spędzoną w Strzelaniu precyzyjnym, możesz powiększyć skuteczny zasięg broni z zasadą zasilaną amunicją wyborową o 1/10. Ilość takich powiększeń nie może być większa niż liczba poziomów w tej umiejętności.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wytrawne oko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jeśli osiągnąłeś 3. poziom tej umiejętności, to modyfikuje zasadę “Dokładne celowanie” podczas strzelania precyzyjnego zmniejszając wymagane przekroczenie rzutu na trafienie z 3 do 2 strzelając z broni z zasadą ?zasilaną amunicją wyborową?. Jeśli posiadasz 6 poziom tej umiejętności to zmniejszasz wymagane przekroczenie rzutu na trafienie z 3 do 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chirurgiczny spust</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każde 2 poziomy tej umiejętności, zwiększ maksymalną premię osiągalną podczas strzelania precyzyjnego o dodatkowe +D6 (wymaga spędzenia dodatkowego czasu w strzelaniu precyzyjnym o wymiarze równym potrzebnemu do uzyskania podstawowych premii).</t>
+  </si>
+  <si>
     <t xml:space="preserve">Luki i kusze</t>
   </si>
   <si>
@@ -173,6 +191,24 @@
     <t xml:space="preserve">łuk, Kusza</t>
   </si>
   <si>
+    <t xml:space="preserve">Sprawne oko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jeśli osiągnąłeś 3. poziom tej umiejętności, to modyfikuje zasadę “Dokładne celowanie” zmniejszając wymagane przekroczenie rzutu na trafienie z 3 do 2 strzelając z łuków i kusz. Jeśli posiadasz 6 poziom tej umiejętności to zmniejszasz wymagane przekroczenie rzutu na trafienie z 3 do 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zdolny strzelec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każdy poziom tej umiejętności zwiększ przyrost zasięgu dla kusz i łuków o 5m.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strzelec wyborowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każdy poziom tej umiejętności zignoruj 10m przy obliczaniu kiedy dojdzie do pierwszego spadku Penetracji przy strzelaniu z łuków i kusz (kolejne spadki Penetracji wciąż następują co 50m).</t>
+  </si>
+  <si>
     <t xml:space="preserve">Materialy wybuchowe</t>
   </si>
   <si>
@@ -182,118 +218,564 @@
     <t xml:space="preserve">Wprawa </t>
   </si>
   <si>
+    <t xml:space="preserve">Granat, Wybuchowa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Analiza trajektorii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każdy poziom tej umiejętności, powiększ przyrost zasięgu granatów o 1m, a skuteczny zasięg granatników o 10m. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">wybuchowy zmysł</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dodatkowa premia do testów umiejętności (nie do testów trafienia, ani testów rzutu granatami) związana ze wszystkimi testami, które mają związek z materiałami wybuchowymi i pirotechniką. Od pułapek, po etapy produkcji. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rzut nad osłoną</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Podczas strzelania z granatnika lub rzutu granatem za każdy poziom umiejętności zmniejszasz o 1 karę wynikającą z osłony, nad którą musisz strzelić/przerzucić ładunek. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Pistolety maszynowe</t>
   </si>
   <si>
     <t xml:space="preserve">obsluga broni, refleks, strzelectwo, zmysl bojowy, ukrywanie, zreczne palce </t>
   </si>
   <si>
+    <t xml:space="preserve">Pistolet maszynowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strzał zza winkla </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jest to dodatkowa premia do testu “zza winkla” podczas strzelania bronią z zasadą Pistolet Maszynowy. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wyczucie naboi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">za każdy poziom tej umiejętności wydłuż zasięg skuteczny broni z zasadą pistolet maszynowy o 20m. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masa robi swoje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeśli podczas strzelania bronią z zasadą Pistolet Maszynowy trafisz większą ilością pocisków niż 2, (np tryb serie, Full Auto) to każdy następny pocisk ma premię do obrażeń +1 względem poprzedniego (trzeci pocisk +1, czwarty pocisk +2,...) </t>
+  </si>
+  <si>
     <t xml:space="preserve">Strzelby</t>
   </si>
   <si>
     <t xml:space="preserve">obsluga broni, refleks, strzelectwo, zmysl bitewny, sprawnosc fizyczna, survival</t>
   </si>
   <si>
+    <t xml:space="preserve">Strzelba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skupienie śrutu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efekty zasady strzelba, zachowują się dalej o liczbę poziomów w tej umiejętności wyrażonej w metrach. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ręczna pompka (Krz/Zr) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Możesz użyć tej umiejętności zamiast walki wręcz podczas strzelania z broni z zasadą specjalną Strzelba. Jeśli wygrasz, wykonujesz normalnie strzał we wroga. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ściana śrutu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeżeli dwa cele stoją dalej niż 5m ale bliżej niż 6m+poziom tej umiejętności od ciebie oraz znajdują się mniej niż 1m od siebie nawzajem, podczas strzelania z broni z zasadą specjalną Strzelba możesz ich obu na raz wziąć za cel. Wykonujesz tylko jeden test ataku z karą -5. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Bojka</t>
   </si>
   <si>
     <t xml:space="preserve">refleks, walka wrecz, zmysl bitewny, ciche poruszanie, sprawnosc fizyczna, survival </t>
   </si>
   <si>
+    <t xml:space="preserve">Trening</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walka Wręcz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Garda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W momencie kiedy w walce wręcz zdecydujesz się bronić, dodaj poziom tej umiejętności do testu walki wręcz. Jeśli przegrasz, po określeniu efektu otrzymanych obrażeń złagodź je o 1 stopień (z śmierci na out of action itd).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dwóch na raz (Zr) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Po sprowadzeniu przeciwnika do stanu ‘out of action’ za pomocą broni białej rzuć ten test. Jeśli wyrzucisz więcej niż 10, możesz w tej samej fazie zadać następny cios, wrogowi w zasięgu. Możesz wykorzystać tą umiejętność tylko raz na fazę </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siła broni białej </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dla broni obuchowej: zwiększa obrażenia z broni podczas uderzenia o liczbę poziomów tej umiejętności. Dla broni tnącej i kłutej: każdy poziom tej umiejętności zwiększa penetrację broni o jeden poziom aż do penetracji ciężkiej.  Następnie, każdy kolejny poziom zwiększa obrażenia o 1.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eliminacja wrecz</t>
   </si>
   <si>
     <t xml:space="preserve">refleks, walka wrecz, zmysł bitewny, ciche poruszanie, sprawnosc fizyczna, zreczne palce </t>
   </si>
   <si>
+    <t xml:space="preserve">Rozbrojenie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tę umiejętność traktujesz jako premię do walki wręcz. Jeśli przeciwnik korzysta z broni do walki wręcz wykonaj test z karą -10. Jeśli Ci się uda- możesz rozbroić przeciwnika nie zadając obrażeń. Kończysz z bronią wroga w ręce (jeśli chcesz i masz wolne ręce) albo broń przeciwnika ląduje na ziemi. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cichy mord (Zr) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jeśli wróg Cię nie widzi ani nie spodziewa, a zdasz ten test na 10, to zabijasz wroga bezszelestnie, gołymi rękoma próg testu jest 15. Garotą na 5. (zauważ że musisz być w kontakcie aby móc to wykonać) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cios ogłuszający </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeśli podczas walki wręcz nie chcesz zranić przeciwnika a jedynie go ogłuszyć nie zadając ran, skorzystaj z ilości poziomów tej umiejętności jako dodatkowego modyfikatora do walki wręcz. Jednocześnie otrzymujesz karę -10. Jeśli wygrasz rzut o nie więcej niż 5 przeciwnik jest oszołomiony (kara -3 do wszystkich testów). Jeśli wygrasz o więcej niż 5 przeciwnik pada na ziemię ogłuszony (czas trwania patrz opis statusu).</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tarcze</t>
   </si>
   <si>
     <t xml:space="preserve">obsluga broni, walka wrecz, sprawnosc fizyczna, survival, zreczne palce, zawod</t>
   </si>
   <si>
+    <t xml:space="preserve">Walka Wręcz, uderzenie tarczą</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ramię ze stali </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każde 2 poziomy tej umiejętności, zwiększ maksymalny bazowy unik wynikający z trzymanej tarczy o 1. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oburęczny </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każdy poziom tej umiejętności zredukuj karę do wykonywania czynności ‘wymagających dwóch rąk’ jedną ręką o 1. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tarczownik </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każdy poziom tej umiejętności powiększ premię do Uniku z wynikającą z tarczy o +1 (nie działa jeśli strzelasz zza tarczy korzystając z celownika, wtedy premia z tarczy staje się premią z osłony częściowej [patrz rozdział 6. Mechanika walki]). </t>
+  </si>
+  <si>
     <t xml:space="preserve">Dowodzenie</t>
   </si>
   <si>
     <t xml:space="preserve">skupienie, zmysl bitewny, spostrzeganie, dyscyplina naukowa lub zawod, gadana, jezyki </t>
   </si>
   <si>
+    <t xml:space="preserve">Autorytet (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeśli sojusznik z jakiegoś powodu się złamał (zabrakło punktów wytrwałości), możesz go przegrupować. Czas trwania takiej akcji to 2 fazy, poziom trudności to ilość punktów wytrwałości na minusie. W wyniku wygranej punkty wytrzymałości regenerowane są do wartości 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ognia! (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wydając rozkaz (poświęcając 1 fazę), jesteś w stanie pomóc jednej osobie kierować ogniem. Progi 5/10/15/20, zapewniają premię 1/2/3/4 do testu trafienia. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZAPOROWY!(int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wydając rozkaz (w tej fazie niz nie zrobisz) zapewniasz premię + 1 do testów strzelectwa ogniem samoczynnym, liczbie osób równą poziomowi tej umiejętności. Dodatkowo zdajesz test. każde 5 teście generuje odebranie dodatkowe 2 PW przeciwnikom ostrzelanym </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Podkomendni </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Możesz posiadać postacie, które będą ci służyły. Ich ilość to liczba poziomów tej umiejętności podzielona przez 3. Każdy ma 100 PU, oraz dostaje ich 2 razy mniej. Każdy może mieć tylko 1 drzewko umiejętności. Posiadają oni własne pieniądze na ekwipunek. (połowę pieniędzy których dostajesz na start) </t>
+  </si>
+  <si>
     <t xml:space="preserve">Pancerz</t>
   </si>
   <si>
     <t xml:space="preserve">walka wrecz, zmysl bojowy, sprawnosc fizyczna, survival, dyscyplina naukowa, zawod </t>
   </si>
   <si>
+    <t xml:space="preserve">Zżyty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każde 2 poziomy tej umiejętności, zwiększ maksymalny bazowy unik w kamizelkach i ochraniaczach o 1. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choinka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każdy poziom tej umiejętności możesz mieć dodatkowy slot k (2k=1A) bez kar do maksymalnego uniku. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dopasowane ochraniacze </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Powiększ premię do uniku wynikającą z posiadania ochraniaczy rąk i nóg o (poziom tej umiejętności)/3 dla ochraniaczy lekkich i (poziom tej umiejętności)/2 dla ochraniaczy ciężkich. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pancernik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każde 2 poziomy tej umiejętności zwiększ redukcję kamizelek o 1. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Szpiegostwo</t>
   </si>
   <si>
     <t xml:space="preserve">ciche poruszanie, spostrzeganie, ukrywanie, zręczne palce, gadana, języki </t>
   </si>
   <si>
+    <t xml:space="preserve">Nietykalny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każde 2 poziomy zainwestowane w tę umiejętność rośnie Bazowy Unik o +1. Traktuj tę premię, jak ze zręczności, więc pamiętaj że kamizelki będą to ograniczać. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">To nie są żołnierze, których szukacie (Int)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeżeli zamierzasz komuś wcisnąć kłamstwo, wtedy możesz skorzystać z tej umiejętności. wynik tej umiejętności to premia do gadany. na 50 przekonujesz żonę, że ta goła pani z łóżka to słynna lekarka, bo potrzebowałeś masażu pleców, a właśnie skończyła, i wgl to że na niej byłeś to nie to co ona myślała, a w ogóle to o co posądzasz głupia babo, TŁUMACZ SIĘ GDZIE BYŁAŚ!!!. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informator(int)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kręcąc się 2 godziny po targu etc, zbierasz informację o danym miejscu. Rzut 20 sprawia że masz wiedzę na poziomie osoby tu mieszkającej (czyli wszystkie zaszłości małżeńskie lokalnej piękności, o menelu co genialnym spawaczem był itd). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doświadczony przemytnik (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dodatkowa Umiejętność której wynik to premia do ukrywania rzeczy przy sobie, i w swoim ekwipunku (plecak itd) oraz do spostrzegania podczas przeszukiwania danego miejsca/osobnika. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Sztuka przetrwania</t>
   </si>
   <si>
     <t xml:space="preserve">skupienie, ciche poruszanie, spostrzeganie, sprawnosc fizyczna, survival, ukrywanie </t>
   </si>
   <si>
+    <t xml:space="preserve">Leśny Sprinter (Zr)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rzut na tę umiejętność określa jak daleko Cię słychać podczas biegu w lesie/ Dżungli. Na 20 słychać Cię w obrębie metra, następnie, każdy 1 rzucony mniej sprawia że słychać Cię w kolejnych 2 m. czyli tak, na 1 słychać Cię w zasięgu 40m. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odtworzenie zdarzeń (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeśli jest to sytuacja poza miejska (Las, obóz itd), to po śladach jesteś w stanie odtworzyć co się stało. Wyniki rzutu 5/10/15/20 do dni 1/2/3/4 wstecz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pułapka (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zdając ten test (5) będąc ukryty, wszystkie czasy w Skupieniu, są skrócone o połowę. Możesz wykorzystać wynik tego testu zamiast ukrywania aby określić czy przeciwnik zdołał cię dostrzec. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mistrz Kamuflażu </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każde 2 poziomy (czy dać poziom) zaokrąglając w dół, dostajesz premię do Uniku, tylko wtedy gdy możesz skorzystać z kamuflażu. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walka w budynku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obsluga broni, refleks, walka wrecz, zmysl bitewny, ciche poruszanie, sprawnosc fizyczna </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każde 2 poziomy tej umiejętności dodaj 1 do wartości Uniku (Bazowego?) podczas gdy jesteś w ruchu. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zejście z linii strzału (Zr) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korzystając z tej umiejętności możesz próbować uzyskać osłonę, w zamian za brak strzelania.Progi 5/10/15/20 uprawniają do premii 1/2/3/4. podczas tej akcji możesz się poruszyć do 2m. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szturmowiec </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każdy poziom umiejętności zwiększ przyrost zasięgu strzelania z biodra, o metr. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wejście </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Podczas wykonywania testów spornych otrzymujesz dodatkowe D6 za każde 2 poziomy tej umiejętności, jeśli jesteś prowokatorem zdarzenia. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dyplomacja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gadana, jezyki, dyscyplina naukowa, skupienie, spostrzeganie, ukrywanie </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wyższe sfery (Int)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Znasz konotacje i powiązania wielkich tego świata, oraz swoich lokalnych. Tą umiejętnością rzuć czy rozpoznajesz jakąś ważną osobę, chociażby lokalną. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Podburzanie (Int </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Możesz przekonać przeciwnika że ktoś jest jego wrogiem. Jest to premia do gadany. Jeśli to jeden z jego kumpli, dzielisz swój wynik przez 3. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dłużnik (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wykonując test tej umiejętności jesteś w stanie przekonać inną osobę do zrobienia rzeczy, której normalnie by nie zrobiła. W zamian za to zaciągasz u niej dług (do kwestii mistrza gry), który prędzej czy później będziesz musiał spłacić lub ponieść konsekwencje. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jest taki jeden (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raz na wioskę/ miasteczko/ dzielnicę możesz rzucić, czy nie znasz jakiegoś wysoko postawioną osobę/ specjalistę. Na 5, znasz pomniejszego specjalistę, kogoś o randze nie wyższej niż sołtysa, 10 wójt bądź jeden z lepszych warsztatów w okolicy, 15 to ktoś o poziomie polityka średniego szczebla, wojewoda, naprawdę dobry specjalista, 20 to już wysokiej klasy fachowcy, ambasadorzy, wiceprezydenci itd, na 25 już prezydent dowolnego kraju, wybitny mistrz danej dziedziny. Pamiętaj że on nie musi Cię najlepiej wspominać. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erudycja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skupienie, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod, gadana, jezyki </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rodzina językowa (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rzuć test tej umiejętności aby spróbować zrozumieć/użyć języka spokrewnionego bądź archaicznego względem jakiegoś który znasz. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Odprawa (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korzystając z tej umiejętności możesz szkolić inne osoby. Wykorzystując kilka godzin możesz tymczasowo zapewnić ilość PU równą testowi tej umiejętności. Aby kogoś wyszkolić, sam musisz posiadać wyższy poziom umiejętności, niż ten którego próbujesz nauczyć. Szkolone umiejętności oraz rozkład PU między członków odprawy definiuje użytkownik. Dotyczy tylko umiejętności inteligenckich. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naukowy Huragan Słów (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skorzystaj z tej umiejętności jeśli chcesz w Naukowy sposób przekonać swojego rozmówcę. Przeciwnik zamiast gadany może wziąć dyscyplinę naukową na odparcie tego ataku słownego. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siła umysłu (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wykonując test tej umiejętności możesz na 1 turę zignorować kary wynikające z posiadanych ran. Poziom trudności testu to [suma kar z ran * 2]. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Handel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spostrzeganie, ukrywanie, dyscyplina naukowa, gadana, jezyki, zawod </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tragarz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Powiększ udźwig o liczbę poziomów tej umiejętności *3 kilogramy. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obyty z kulturą (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rzucając na tę umiejętność jesteś w stanie sobie przypomnieć lokalne zwyczaje. 5 dla lokalizacji które odwiedziłeś wielokrotnie, 30 jeśli czytałeś tylko przewodnik i nigdy tam nie byłeś. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pokaż mi swoje towary (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rzuć na tę umiejętność za każdym razem kiedy masz problem ze znalezieniem towaru (np bardzo rzadkich naboi SP-6). Jeśli zdasz ten test (w tym przypadku poziom trudności 15) zaraz się okaże, że może i handlarz nie ma, za to kumpel jego kumpla co siedzi tam w namiocie chyba coś ma. Rzuciłeś 20? No to ten kolega ma. Całe 150 sztuk. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobijanie targu (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Masz zmysł kupiecki na szóstkę z plusem. Za każdym razem jak wymyślisz dobry argument do zbicia ceny zastosuj go. Jeśli Ci się uda (najczęściej poziom trudności będzie od 5 dla zwykłego człeka, 15 dla lepszego sprzedawcy, do 20 dla bankiera) zabijasz cenę o ⅕ do wartości rynkowej. Jak dojdziesz do wartości rynkowej może się okazać, że za więcej będzie trudno. Tak samo jak ktoś za tanio od Ciebie chcę skupić, tylko tym razem za każdy zdany test cena idzie w górę o ⅕ (w zależności od argumentu może być więcej lub mniej). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medycyna polowa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skupienie, survival, zreczne palce, dyscyplina naukowa, dyscyplina naukowa, gadana </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szybciej, on umiera (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daje Ci możliwość opatrzenia rany w połowę czasu. Jest to rzut jak na Dyscyplina Naukowa (Medycyna), ale jest on 2 razy trudniejszy (ale dodajesz wynik rzutu na tę umiejętność jako premię). Korzystając z tej umiejętności nie korzystasz z premii z Predyspozycji do dyscypliny naukowej. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Szeroki bandaż </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każde 2 poziomy tej umiejętności możesz opatrywać 1 dodatkową ranę podczas tego samego testu leczenia. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Improwizowane medykamenty </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skorzystaj z tego jako premia do survivalu, jak szukasz medykamentów, w wysokości poziom tej umiejętności *5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Powstań(Zr) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za pomocą tej umiejętności zdajesz i wykonujesz akcję Bardzo szybką: wyjęcie z ładownicy i zaaplikowanie adrenaliny(w jednej akcji). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motoryzacja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skupienie, prowadzenie pojazdu, spostrzeganie, zręczne palce, dyscyplina naukowa, zawod Mechanik </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ekspert Mechaniki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Widząc silnik odpala Ci się rozumienie ponadprzeciętne. jest to premia do wszystkich testów (poza prowadzeniem) związanymi z silnikami, hamulcami i zawieszeniem. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rajdowiec </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zmniejsza karę do testów jazdy terenowej o liczbę poziomów w tej umiejętności (tak przy prostych czynnościach zapewnia premię). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gaz i Strzał (Zr) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">???????????</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uliczny Wirtuoz (Zr) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Podczas prowadzenia pojazdu, jeśli chcesz robić coś, co jest jeszcze zgodne z prawami fizyki, ale wymaga niesłychanie wielkiej umiejętności, gdzie na prowadzenie pojazdu byłoby bardzo trudno zdać, dorzuć sobie tą umiejętność. wynik rzutu na tę umiejętność to premia do testu kierowania pojazdem. Nie możesz jednocześnie używać tej umiejętności oraz Gaz i Strzał. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nauka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skupienie, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod, jezyki </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teoria w praktyce (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dodatkowa premia (tak jest to umiejętność więc premia jest wysoka) w momencie kiedy chcesz ustawić pułapkę, bądź rozbroić pułapkę. Może być również używane w celu znalezienia słabych punktów konstrukcyjnych budynków, w celu ich zawalenia. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mistrz biochemii (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z sekcji zwłok, jesteś w stanie uzyskać bardziej szczegółowe informacje o przeciwniku. Możesz to traktować jako oddzielną umiejętność, ALBO premię do rzutu (np. dyscyplina naukowa: biologia/medycyna). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mprowizowane przyrządy pomiarowe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bez specjalistycznej aparatury nie zrobisz sekwencjonowania DNA, ale ten nóż jest niezłym skalpelem. Premia do użycia za każdym razem kiedy chciałbyś mieć specjalistyczne narzędzia do danej czynności pomiarowej ale ich nie masz. Odpowiednie otoczenie, również zapewnia premię do tego rzutu (ooo ten celownik to niezły teleskop jest itd). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logiczny szturm (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeśli masz 2 poziomy umiejętności w danym zawodzie/dyscyplinie naukowej, to możesz dorzucić wynik tego testu jako premia. aby móc dorzucić musisz złapać spokój, posłuchać ulubionej piosenki itd. Około 10 minut musisz się skupiać nad danym problemem/relaksować się myśląc o nim (co pochłania CAŁĄ Twoją uwagę). Na 50 odkrywasz błąd, który każdy przeoczył, w Kernelu OSa, który umożliwia CI przejęcie pełnej kontroli nad sprzętem. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prowizorka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skupienie, prowadzenie pojazdu, zreczne palce, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chwilowe rozwiązanie </t>
+  </si>
+  <si>
+    <t xml:space="preserve">jeśli wykonujesz test zakładający modyfikację lub naprawę obiektu bądź jego zawartości (dotyczy też oprogramowania) i wyrzucisz poniżej poziomu trudności, ale przynajmniej [poziom trudności - 2*Prowizorka] twoja akcja kończy się tymczasowym powodzeniem. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Części zapasowe (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Za każdym razem, gdy potrzebujesz jakiejś drobnej części do naprawy sprzętu, rzuć na tę umiejętność. Progi 5/10/15/20 uprawniają cię do znalezienia w swoim ekwipunku coraz to bardziej wymyślnych części (od wtyczki za 5, po kostkę Winbond Q25, a akurat taka uległa uszkodzeniu…) o ile jest to fabularnie możliwe. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Działanie pod presją </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Każdy poziom tej umiejętności dodaje premię +1 do testu Skupienia wykonywanego podczas jednoczesnej naprawy/modyfikacji/manipulacji oraz prowadzenia ostrzału. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neutralizacja (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strzelając do jakiegokolwiek sprzętu (pojazd, komputer, itd.) wykonaj test tej umiejętności po udanym trafieniu (pod warunkiem że test trafienia przewyższył unik przeciwnika o 3). Jeśli uda ci się ten test uszkadzasz sprzęt w sposób uniemożliwiający dalsze działanie bez całkowitego zniszczenia go. Poziom trudności określa mistrz gry (5 dla powszechnej maszyny( pojazd etc,) 10 dla znanego komputera, 15 dla UAVa). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Technologia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skupienie, prowadzenie pojazdu, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pełne skupienie </t>
+  </si>
+  <si>
+    <t xml:space="preserve">W momencie kiedy wziąłeś sobie za punkt honoru rozwiązać daną zagadkę logiczno- naukową otrzymujesz dodatkową premię, w wysokości poziomów tej umiejętności. Aby z tego skorzystać musisz spokojnie usiąść, i nikt przez turę nie może Ci przeszkadzać (Test skupienia 10 za każdy pomruk) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zdalna kontrola </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dodatkowa premia do wszystkich testów urządzeń zdalnych, od robotów, po drony. Nawet do zwykłego serwera. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hack &amp; slash (Zr) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jak zdasz ten test to możesz bez przerywania czynności którą jesteś w stanie wykonywać jedną ręką, prowadzić ogień z 2 ręki. Działa jak premia do skupienia, oraz umożliwia wykonanie tego testu (10). Jeśli zdasz test, możesz kontynuować </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mistrz szyfrów (Int) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wynik rzutu tej umiejętności to dodatkowa premia za każdym razem gdy masz do czynienia z kodowaniem/szyfrowaniem danych. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Uniwersalista</t>
   </si>
   <si>
     <t xml:space="preserve">obsluga broni, strzelectwo, refleks, zmysł bitewny, spostrzeganie, zreczne palce </t>
   </si>
   <si>
-    <t xml:space="preserve">Walka w budynku</t>
-  </si>
-  <si>
-    <t xml:space="preserve">obsluga broni, refleks, walka wrecz, zmysl bitewny, ciche poruszanie, sprawnosc fizyczna </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dyplomacja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gadana, jezyki, dyscyplina naukowa, skupienie, spostrzeganie, ukrywanie </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erudycja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skupienie, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod, gadana, jezyki </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Handel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spostrzeganie, ukrywanie, dyscyplina naukowa, gadana, jezyki, zawod </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medycyna polowa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skupienie, survival, zreczne palce, dyscyplina naukowa, dyscyplina naukowa, gadana </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Motoryzacja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skupienie, prowadzenie pojazdu, spostrzeganie, zręczne palce, dyscyplina naukowa, zawod Mechanik </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nauka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skupienie, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod, jezyki </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prowizorka</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skupienie, prowadzenie pojazdu, zreczne palce, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Technologia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skupienie, prowadzenie pojazdu, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod, dyscyplina naukowa lub zawod,</t>
+    <t xml:space="preserve">Wprawa
+Możesz zamienić wynik wyrzucony na jednej z kości podczas testu Zręcznych palców bądź Strzelectwa na liczbę równą poziomowi tej umiejętności podczas strzelania odpowiednio z łuku lub kuszy. Nie łączy się z umiejętnościami o tej samej nazwie z innych specjalizacji.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.Predyspozycje
+Poziom tej umiejętności dodajesz jako bonus do wyników testów umiejętności powiązanych.</t>
   </si>
 </sst>
 </file>
@@ -303,7 +785,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -356,6 +838,13 @@
       <family val="1"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -402,7 +891,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -431,8 +920,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -453,13 +962,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U29"/>
+  <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N26" activeCellId="0" sqref="N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="97.56"/>
@@ -699,7 +1208,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -718,19 +1227,37 @@
       <c r="F6" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="I6" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="L6" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>0</v>
@@ -739,411 +1266,873 @@
         <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G7" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="I7" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J7" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="L7" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M7" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C8" s="3" t="n">
         <v>0</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>52</v>
+        <v>64</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G8" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="I8" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J8" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="L8" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M8" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>0</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>52</v>
+        <v>64</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>74</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G9" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="I9" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J9" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="L9" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M9" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D10" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>83</v>
+      </c>
       <c r="F10" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G10" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="I10" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J10" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="L10" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M10" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D11" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>93</v>
+      </c>
       <c r="F11" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G11" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>95</v>
+      </c>
       <c r="I11" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J11" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="L11" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M11" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D12" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>93</v>
+      </c>
       <c r="F12" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G12" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="I12" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J12" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="L12" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M12" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>108</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D13" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>110</v>
+      </c>
       <c r="F13" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G13" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="I13" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J13" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="L13" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M13" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D14" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="F14" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G14" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="I14" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J14" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>124</v>
+      </c>
       <c r="L14" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M14" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D15" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>130</v>
+      </c>
       <c r="F15" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G15" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="I15" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J15" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>134</v>
+      </c>
       <c r="L15" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="8.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="M15" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>67</v>
+        <v>137</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>68</v>
+        <v>138</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D16" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F16" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G16" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="I16" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J16" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>144</v>
+      </c>
       <c r="L16" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M16" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>69</v>
+        <v>147</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>148</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D17" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="F17" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G17" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>152</v>
+      </c>
       <c r="I17" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J17" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>154</v>
+      </c>
       <c r="L17" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>71</v>
+      <c r="M17" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
+        <v>157</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>72</v>
+        <v>158</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D18" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>160</v>
+      </c>
       <c r="F18" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G18" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="I18" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J18" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>164</v>
+      </c>
       <c r="L18" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
-        <v>73</v>
+      <c r="M18" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
       <c r="C19" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D19" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>170</v>
+      </c>
       <c r="F19" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G19" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="I19" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J19" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>174</v>
+      </c>
       <c r="L19" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M19" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>75</v>
+        <v>177</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>76</v>
+        <v>178</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D20" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="F20" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G20" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>182</v>
+      </c>
       <c r="I20" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J20" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>184</v>
+      </c>
       <c r="L20" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M20" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>77</v>
+        <v>187</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>78</v>
+        <v>188</v>
       </c>
       <c r="C21" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D21" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>190</v>
+      </c>
       <c r="F21" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G21" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>192</v>
+      </c>
       <c r="I21" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J21" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>194</v>
+      </c>
       <c r="L21" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M21" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>79</v>
+        <v>197</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>80</v>
+        <v>198</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D22" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>200</v>
+      </c>
       <c r="F22" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G22" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>202</v>
+      </c>
       <c r="I22" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J22" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>204</v>
+      </c>
       <c r="L22" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>81</v>
+      <c r="M22" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
+        <v>207</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>82</v>
+        <v>208</v>
       </c>
       <c r="C23" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D23" s="0" t="s">
+        <v>209</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>210</v>
+      </c>
       <c r="F23" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G23" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>212</v>
+      </c>
       <c r="I23" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J23" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>214</v>
+      </c>
       <c r="L23" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>84</v>
+      <c r="M23" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>218</v>
       </c>
       <c r="C24" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D24" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>220</v>
+      </c>
       <c r="F24" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G24" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>222</v>
+      </c>
       <c r="I24" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J24" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>224</v>
+      </c>
       <c r="L24" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M24" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>85</v>
+        <v>227</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>86</v>
+        <v>228</v>
       </c>
       <c r="C25" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D25" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>230</v>
+      </c>
       <c r="F25" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G25" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>232</v>
+      </c>
       <c r="I25" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J25" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>234</v>
+      </c>
       <c r="L25" s="3" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>87</v>
+      <c r="M25" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>237</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>88</v>
+        <v>238</v>
       </c>
       <c r="C26" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="D26" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>240</v>
+      </c>
       <c r="F26" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="G26" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>242</v>
+      </c>
       <c r="I26" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="J26" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>244</v>
+      </c>
       <c r="L26" s="3" t="n">
         <v>0</v>
       </c>
+      <c r="M26" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="C27" s="3" t="n">
         <v>0</v>
       </c>
@@ -1171,19 +2160,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I29" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L29" s="3" t="n">
-        <v>0</v>
-      </c>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="10"/>
+    </row>
+    <row r="37" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="11"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>